<commit_message>
CHG: Projektplan und Riskmanagement aktualisiert
</commit_message>
<xml_diff>
--- a/Documentation/Risikomanagement/RiskManagement.xlsx
+++ b/Documentation/Risikomanagement/RiskManagement.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
   <si>
     <t>Identified</t>
   </si>
@@ -117,6 +117,18 @@
   </si>
   <si>
     <t>Neuinstallation, anderen Gruppen fragen</t>
+  </si>
+  <si>
+    <t>mangelnde Fehlerfindung wegen fehlender Tests</t>
+  </si>
+  <si>
+    <t>Höhere Priorisierung der Tests</t>
+  </si>
+  <si>
+    <t>sehr viel Zeit für Refactoring</t>
+  </si>
+  <si>
+    <t>vor der Implementierung informieren</t>
   </si>
 </sst>
 </file>
@@ -256,10 +268,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A3:F14" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A3:F14"/>
-  <sortState ref="A4:F14">
-    <sortCondition descending="1" ref="B3:B14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A3:F16" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A3:F16"/>
+  <sortState ref="A4:F16">
+    <sortCondition descending="1" ref="B3:B16"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" name="Identified" dataDxfId="5"/>
@@ -565,10 +577,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,85 +661,85 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="4">
-        <f>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</f>
-        <v>5.2</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0.65</v>
+        <v>32</v>
+      </c>
+      <c r="B6" s="7">
+        <f>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</f>
+        <v>5.6</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0.7</v>
       </c>
       <c r="D6" s="4">
         <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="4">
+        <f>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</f>
+        <v>5.2</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0.65</v>
+      </c>
+      <c r="D7" s="4">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B8" s="4">
         <f>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</f>
         <v>4.5</v>
-      </c>
-      <c r="C7" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="D7" s="4">
-        <v>9</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="4">
-        <f>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</f>
-        <v>3.5</v>
       </c>
       <c r="C8" s="5">
         <v>0.5</v>
       </c>
       <c r="D8" s="4">
+        <v>9</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4">
+        <f>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</f>
+        <v>3.5</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="4">
         <v>7</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="7">
-        <f>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</f>
-        <v>1</v>
-      </c>
-      <c r="C9" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="D9" s="4">
-        <v>5</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>27</v>
@@ -739,10 +751,10 @@
       </c>
       <c r="B10" s="4">
         <f>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</f>
-        <v>0.70000000000000007</v>
+        <v>2.8000000000000003</v>
       </c>
       <c r="C10" s="5">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="D10" s="4">
         <v>7</v>
@@ -756,85 +768,127 @@
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="4">
-        <f>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</f>
-        <v>0.60000000000000009</v>
-      </c>
-      <c r="C11" s="5">
-        <v>0.1</v>
+        <v>34</v>
+      </c>
+      <c r="B11" s="7">
+        <f>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</f>
+        <v>2.4</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.6</v>
       </c>
       <c r="D11" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="4">
-        <f>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</f>
-        <v>0.4</v>
-      </c>
-      <c r="C12" s="5">
+        <v>30</v>
+      </c>
+      <c r="B12" s="7">
+        <f>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</f>
+        <v>1</v>
+      </c>
+      <c r="C12" s="8">
         <v>0.2</v>
       </c>
       <c r="D12" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B13" s="4">
         <f>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</f>
-        <v>0.2</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="C13" s="5">
         <v>0.1</v>
       </c>
       <c r="D13" s="4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="4">
+        <f>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</f>
+        <v>0.4</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="D14" s="4">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="4">
+        <f>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</f>
+        <v>0.2</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="D15" s="4">
+        <v>2</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B16" s="4">
         <f>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</f>
         <v>0.15000000000000002</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C16" s="5">
         <v>0.05</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D16" s="4">
         <v>3</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>